<commit_message>
Update Report Tuan 4
</commit_message>
<xml_diff>
--- a/Report/SmartRecycleBin_Timeline_20220405_20220502.xlsx
+++ b/Report/SmartRecycleBin_Timeline_20220405_20220502.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Projects\MyWork\ThungRacThongMinh\SmartRecycleBin\Document\OldFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My_data\SmartRecycleBin\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EDFAC1-4218-4642-9100-BE619695189F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B865A273-A0E2-462F-8526-C13B26897FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Start</t>
   </si>
@@ -79,10 +79,16 @@
     <t>Lập trình tính năng.</t>
   </si>
   <si>
-    <t>Thử nghiệm tính năng và demo lần 1.</t>
+    <t>Gia công cơ khí.</t>
   </si>
   <si>
-    <t>Thử nghiệm demo lần 2.</t>
+    <t>Kết hợp mạch với cơ khí.</t>
+  </si>
+  <si>
+    <t>Thử nghiệm demo lần 1.</t>
+  </si>
+  <si>
+    <t>Thử nghiệm lần 2.</t>
   </si>
 </sst>
 </file>
@@ -130,13 +136,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color theme="0"/>
@@ -158,6 +157,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -291,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -306,56 +313,67 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1234,17 +1252,18 @@
       <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E51" sqref="E51"/>
+      <selection pane="bottomRight" activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" customWidth="1"/>
-    <col min="6" max="8" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" style="32" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="7" max="8" width="9.28515625" customWidth="1"/>
     <col min="9" max="9" width="3" customWidth="1"/>
     <col min="10" max="10" width="2.7109375" customWidth="1"/>
     <col min="11" max="12" width="2.7109375" style="1" customWidth="1"/>
@@ -1267,34 +1286,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:117" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
       <c r="F1" s="11"/>
     </row>
-    <row r="2" spans="1:117" s="6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="1:117" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="33">
         <f>DATE(2022, 4, 5)</f>
         <v>44656</v>
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:117" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:117" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="33">
         <f ca="1">IF(D3&lt;&gt;"",D3,TODAY())</f>
-        <v>44663</v>
-      </c>
-      <c r="D3" s="15"/>
+        <v>44670</v>
+      </c>
+      <c r="D3" s="14"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
@@ -1542,271 +1561,271 @@
     </row>
     <row r="4" spans="1:117" s="4" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
-      <c r="I4" s="19" t="str">
+      <c r="I4" s="16" t="str">
         <f>TEXT(I5,"MMM")</f>
         <v>Apr</v>
       </c>
-      <c r="J4" s="19" t="str">
+      <c r="J4" s="16" t="str">
         <f>TEXT(J5,"MMM")</f>
         <v>Apr</v>
       </c>
-      <c r="K4" s="19" t="str">
+      <c r="K4" s="16" t="str">
         <f>TEXT(K5,"MMM")</f>
         <v>Apr</v>
       </c>
-      <c r="L4" s="19" t="str">
+      <c r="L4" s="16" t="str">
         <f t="shared" ref="L4:AM4" si="1">TEXT(L5,"MMM")</f>
         <v>Apr</v>
       </c>
-      <c r="M4" s="19" t="str">
+      <c r="M4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="N4" s="19" t="str">
+      <c r="N4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="O4" s="19" t="str">
+      <c r="O4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="P4" s="19" t="str">
+      <c r="P4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="Q4" s="19" t="str">
+      <c r="Q4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="R4" s="19" t="str">
+      <c r="R4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="S4" s="19" t="str">
+      <c r="S4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="T4" s="19" t="str">
+      <c r="T4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="U4" s="19" t="str">
+      <c r="U4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="V4" s="19" t="str">
+      <c r="V4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="W4" s="19" t="str">
+      <c r="W4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="X4" s="19" t="str">
+      <c r="X4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="Y4" s="19" t="str">
+      <c r="Y4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="Z4" s="19" t="str">
+      <c r="Z4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="AA4" s="19" t="str">
+      <c r="AA4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="AB4" s="19" t="str">
+      <c r="AB4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="AC4" s="19" t="str">
+      <c r="AC4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="AD4" s="19" t="str">
+      <c r="AD4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="AE4" s="19" t="str">
+      <c r="AE4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="AF4" s="19" t="str">
+      <c r="AF4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="AG4" s="19" t="str">
+      <c r="AG4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="AH4" s="19" t="str">
+      <c r="AH4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="AI4" s="19" t="str">
+      <c r="AI4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="AJ4" s="19" t="str">
+      <c r="AJ4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="AK4" s="19" t="str">
+      <c r="AK4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="AL4" s="19" t="str">
+      <c r="AL4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="AM4" s="19" t="str">
+      <c r="AM4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="AN4" s="19" t="str">
+      <c r="AN4" s="16" t="str">
         <f t="shared" ref="AN4:BO4" si="2">TEXT(AN5,"MMM")</f>
         <v>May</v>
       </c>
-      <c r="AO4" s="19" t="str">
+      <c r="AO4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="AP4" s="19" t="str">
+      <c r="AP4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="AQ4" s="19" t="str">
+      <c r="AQ4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="AR4" s="19" t="str">
+      <c r="AR4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="AS4" s="19" t="str">
+      <c r="AS4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="AT4" s="19" t="str">
+      <c r="AT4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="AU4" s="19" t="str">
+      <c r="AU4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="AV4" s="19" t="str">
+      <c r="AV4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="AW4" s="19" t="str">
+      <c r="AW4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="AX4" s="19" t="str">
+      <c r="AX4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="AY4" s="19" t="str">
+      <c r="AY4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="AZ4" s="19" t="str">
+      <c r="AZ4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="BA4" s="19" t="str">
+      <c r="BA4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="BB4" s="19" t="str">
+      <c r="BB4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="BC4" s="19" t="str">
+      <c r="BC4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="BD4" s="19" t="str">
+      <c r="BD4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="BE4" s="19" t="str">
+      <c r="BE4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="BF4" s="19" t="str">
+      <c r="BF4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="BG4" s="19" t="str">
+      <c r="BG4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="BH4" s="19" t="str">
+      <c r="BH4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="BI4" s="19" t="str">
+      <c r="BI4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="BJ4" s="19" t="str">
+      <c r="BJ4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="BK4" s="19" t="str">
+      <c r="BK4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="BL4" s="19" t="str">
+      <c r="BL4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="BM4" s="19" t="str">
+      <c r="BM4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="BN4" s="19" t="str">
+      <c r="BN4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="BO4" s="19" t="str">
+      <c r="BO4" s="16" t="str">
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
     </row>
     <row r="5" spans="1:117" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="15" t="s">
         <v>1</v>
       </c>
       <c r="I5" s="9">
@@ -2248,25 +2267,25 @@
     </row>
     <row r="6" spans="1:117" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="30" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="18">
         <f>C2+1</f>
         <v>44657</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="18">
         <f>F6+4</f>
         <v>44661</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="18">
         <f>F6+6</f>
         <v>44663</v>
       </c>
@@ -2344,13 +2363,13 @@
     </row>
     <row r="7" spans="1:117" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
       <c r="I7" s="7" t="str">
         <f t="shared" ref="I7:BO7" si="5">IF(AND(I$5&gt;=$F6,I$5&lt;=$G6),1,"")</f>
         <v/>
@@ -2602,13 +2621,13 @@
     </row>
     <row r="8" spans="1:117" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
       <c r="I8" s="7" t="str">
         <f t="shared" ref="I8:AN8" ca="1" si="6">IF(OR($H6&gt;I$5,$H6=""),IF(AND(I$5&gt;=$F6,I$5&lt;=$C$3),2,IF(AND(I$5&gt;=$F6,I$5&lt;=$G6),1,"")), IF($H6=I$5,3,I9))</f>
         <v/>
@@ -2860,13 +2879,13 @@
     </row>
     <row r="9" spans="1:117" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
       <c r="I9" s="8" t="str">
         <f t="shared" ref="I9:BB9" si="8">IF(AND(I$5&gt;=$F6,I$5&lt;=$G6),1,"")</f>
         <v/>
@@ -3118,21 +3137,21 @@
     </row>
     <row r="10" spans="1:117" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="24" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="18">
         <f>C2+3</f>
         <v>44659</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="18">
         <f>F10+3</f>
         <v>44662</v>
       </c>
-      <c r="H10" s="27">
+      <c r="H10" s="18">
         <f>F10</f>
         <v>44659</v>
       </c>
@@ -3210,13 +3229,13 @@
     </row>
     <row r="11" spans="1:117" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
       <c r="I11" s="7" t="str">
         <f t="shared" ref="I11:AN11" si="10">IF(AND(I$5&gt;=$F10,I$5&lt;=$G10),1,"")</f>
         <v/>
@@ -3468,13 +3487,13 @@
     </row>
     <row r="12" spans="1:117" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
       <c r="I12" s="7" t="str">
         <f t="shared" ref="I12:AN12" ca="1" si="12">IF(OR($H10&gt;I$5,$H10=""),IF(AND(I$5&gt;=$F10,I$5&lt;=$C$3),2,IF(AND(I$5&gt;=$F10,I$5&lt;=$G10),1,"")), IF($H10=I$5,3,I13))</f>
         <v/>
@@ -3726,13 +3745,13 @@
     </row>
     <row r="13" spans="1:117" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
       <c r="I13" s="8" t="str">
         <f t="shared" ref="I13:BB13" si="14">IF(AND(I$5&gt;=$F10,I$5&lt;=$G10),1,"")</f>
         <v/>
@@ -3984,23 +4003,23 @@
     </row>
     <row r="14" spans="1:117" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="24" t="s">
+      <c r="B14" s="28"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="18">
         <f>C2+4</f>
         <v>44660</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="18">
         <f>F14+6</f>
         <v>44666</v>
       </c>
-      <c r="H14" s="27">
-        <f>F14+6</f>
-        <v>44666</v>
+      <c r="H14" s="18">
+        <f>F14+7</f>
+        <v>44667</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
@@ -4076,13 +4095,13 @@
     </row>
     <row r="15" spans="1:117" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
       <c r="I15" s="7" t="str">
         <f t="shared" ref="I15:AN15" si="16">IF(AND(I$5&gt;=$F14,I$5&lt;=$G14),1,"")</f>
         <v/>
@@ -4334,13 +4353,13 @@
     </row>
     <row r="16" spans="1:117" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
       <c r="I16" s="7" t="str">
         <f t="shared" ref="I16:AN16" ca="1" si="18">IF(OR($H14&gt;I$5,$H14=""),IF(AND(I$5&gt;=$F14,I$5&lt;=$C$3),2,IF(AND(I$5&gt;=$F14,I$5&lt;=$G14),1,"")), IF($H14=I$5,3,I17))</f>
         <v/>
@@ -4375,19 +4394,19 @@
       </c>
       <c r="Q16" s="7">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R16" s="7">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S16" s="7">
+        <f t="shared" ca="1" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="T16" s="7">
         <f t="shared" si="18"/>
         <v>3</v>
-      </c>
-      <c r="T16" s="7" t="str">
-        <f t="shared" si="18"/>
-        <v/>
       </c>
       <c r="U16" s="7" t="str">
         <f t="shared" si="18"/>
@@ -4592,13 +4611,13 @@
     </row>
     <row r="17" spans="1:79" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
       <c r="I17" s="8" t="str">
         <f t="shared" ref="I17:BB17" si="20">IF(AND(I$5&gt;=$F14,I$5&lt;=$G14),1,"")</f>
         <v/>
@@ -4850,21 +4869,21 @@
     </row>
     <row r="18" spans="1:79" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="24" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="18">
         <f>C2+4</f>
         <v>44660</v>
       </c>
-      <c r="G18" s="27">
-        <f>F18+8</f>
-        <v>44668</v>
-      </c>
-      <c r="H18" s="27"/>
+      <c r="G18" s="18">
+        <f>F18+20</f>
+        <v>44680</v>
+      </c>
+      <c r="H18" s="18"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
@@ -4939,13 +4958,13 @@
     </row>
     <row r="19" spans="1:79" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
       <c r="I19" s="7" t="str">
         <f t="shared" ref="I19:AN19" si="22">IF(AND(I$5&gt;=$F18,I$5&lt;=$G18),1,"")</f>
         <v/>
@@ -4998,53 +5017,53 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="V19" s="7" t="str">
+      <c r="V19" s="7">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="W19" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="W19" s="7">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="X19" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="X19" s="7">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="Y19" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="7">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="Z19" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="7">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="AA19" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="7">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="AB19" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AB19" s="7">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="AC19" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AC19" s="7">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="AD19" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AD19" s="7">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="AE19" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AE19" s="7">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="AF19" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AF19" s="7">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="AG19" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AG19" s="7">
         <f t="shared" si="22"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AH19" s="7" t="str">
         <f t="shared" si="22"/>
@@ -5197,13 +5216,13 @@
     </row>
     <row r="20" spans="1:79" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
       <c r="I20" s="7" t="str">
         <f t="shared" ref="I20:AN20" ca="1" si="24">IF(OR($H18&gt;I$5,$H18=""),IF(AND(I$5&gt;=$F18,I$5&lt;=$C$3),2,IF(AND(I$5&gt;=$F18,I$5&lt;=$G18),1,"")), IF($H18=I$5,3,I21))</f>
         <v/>
@@ -5238,71 +5257,71 @@
       </c>
       <c r="Q20" s="7">
         <f t="shared" ca="1" si="24"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R20" s="7">
         <f t="shared" ca="1" si="24"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S20" s="7">
         <f t="shared" ca="1" si="24"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T20" s="7">
         <f t="shared" ca="1" si="24"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U20" s="7">
         <f t="shared" ca="1" si="24"/>
-        <v>1</v>
-      </c>
-      <c r="V20" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="V20" s="7">
         <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="W20" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="W20" s="7">
         <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="X20" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="X20" s="7">
         <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="Y20" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="7">
         <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="Z20" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="7">
         <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AA20" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="7">
         <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AB20" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="7">
         <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AC20" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="7">
         <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AD20" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AD20" s="7">
         <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AE20" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="7">
         <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AF20" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AF20" s="7">
         <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AG20" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AG20" s="7">
         <f t="shared" ca="1" si="24"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AH20" s="7" t="str">
         <f t="shared" ca="1" si="24"/>
@@ -5455,13 +5474,13 @@
     </row>
     <row r="21" spans="1:79" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
       <c r="I21" s="8" t="str">
         <f t="shared" ref="I21:BB21" si="26">IF(AND(I$5&gt;=$F18,I$5&lt;=$G18),1,"")</f>
         <v/>
@@ -5514,53 +5533,53 @@
         <f t="shared" si="26"/>
         <v>1</v>
       </c>
-      <c r="V21" s="8" t="str">
+      <c r="V21" s="8">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="W21" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="W21" s="8">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="X21" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="X21" s="8">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="Y21" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="8">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="Z21" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="8">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="AA21" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="8">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="AB21" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="8">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="AC21" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="8">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="AD21" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="AD21" s="8">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="AE21" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="AE21" s="8">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="AF21" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="AF21" s="8">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="AG21" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="AG21" s="8">
         <f t="shared" si="26"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AH21" s="8" t="str">
         <f t="shared" si="26"/>
@@ -5713,21 +5732,21 @@
     </row>
     <row r="22" spans="1:79" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="24" t="s">
+      <c r="B22" s="28"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="27">
-        <f>C2+5</f>
-        <v>44661</v>
-      </c>
-      <c r="G22" s="27">
-        <f>F22+10</f>
-        <v>44671</v>
-      </c>
-      <c r="H22" s="27"/>
+      <c r="F22" s="18">
+        <f>C2+10</f>
+        <v>44666</v>
+      </c>
+      <c r="G22" s="18">
+        <f>F22+7</f>
+        <v>44673</v>
+      </c>
+      <c r="H22" s="18"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
@@ -5802,13 +5821,13 @@
     </row>
     <row r="23" spans="1:79" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
       <c r="I23" s="7" t="str">
         <f t="shared" ref="I23:AN23" si="28">IF(AND(I$5&gt;=$F22,I$5&lt;=$G22),1,"")</f>
         <v/>
@@ -5829,25 +5848,25 @@
         <f t="shared" si="28"/>
         <v/>
       </c>
-      <c r="N23" s="7">
+      <c r="N23" s="7" t="str">
         <f t="shared" si="28"/>
-        <v>1</v>
-      </c>
-      <c r="O23" s="7">
+        <v/>
+      </c>
+      <c r="O23" s="7" t="str">
         <f t="shared" si="28"/>
-        <v>1</v>
-      </c>
-      <c r="P23" s="7">
+        <v/>
+      </c>
+      <c r="P23" s="7" t="str">
         <f t="shared" si="28"/>
-        <v>1</v>
-      </c>
-      <c r="Q23" s="7">
+        <v/>
+      </c>
+      <c r="Q23" s="7" t="str">
         <f t="shared" si="28"/>
-        <v>1</v>
-      </c>
-      <c r="R23" s="7">
+        <v/>
+      </c>
+      <c r="R23" s="7" t="str">
         <f t="shared" si="28"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="S23" s="7">
         <f t="shared" si="28"/>
@@ -5873,13 +5892,13 @@
         <f t="shared" si="28"/>
         <v>1</v>
       </c>
-      <c r="Y23" s="7" t="str">
+      <c r="Y23" s="7">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="Z23" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="7">
         <f t="shared" si="28"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AA23" s="7" t="str">
         <f t="shared" si="28"/>
@@ -6060,13 +6079,13 @@
     </row>
     <row r="24" spans="1:79" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
       <c r="I24" s="7" t="str">
         <f t="shared" ref="I24:AN24" ca="1" si="30">IF(OR($H22&gt;I$5,$H22=""),IF(AND(I$5&gt;=$F22,I$5&lt;=$C$3),2,IF(AND(I$5&gt;=$F22,I$5&lt;=$G22),1,"")), IF($H22=I$5,3,I25))</f>
         <v/>
@@ -6087,57 +6106,57 @@
         <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
-      <c r="N24" s="7">
+      <c r="N24" s="7" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="O24" s="7" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="P24" s="7" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="Q24" s="7" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="R24" s="7" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="S24" s="7">
         <f t="shared" ca="1" si="30"/>
         <v>2</v>
       </c>
-      <c r="O24" s="7">
+      <c r="T24" s="7">
         <f t="shared" ca="1" si="30"/>
         <v>2</v>
       </c>
-      <c r="P24" s="7">
+      <c r="U24" s="7">
         <f t="shared" ca="1" si="30"/>
         <v>2</v>
       </c>
-      <c r="Q24" s="7">
-        <f t="shared" ca="1" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="R24" s="7">
-        <f t="shared" ca="1" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="S24" s="7">
-        <f t="shared" ca="1" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="T24" s="7">
-        <f t="shared" ca="1" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="U24" s="7">
-        <f t="shared" ca="1" si="30"/>
-        <v>1</v>
-      </c>
       <c r="V24" s="7">
         <f t="shared" ca="1" si="30"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W24" s="7">
         <f t="shared" ca="1" si="30"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X24" s="7">
         <f t="shared" ca="1" si="30"/>
         <v>1</v>
       </c>
-      <c r="Y24" s="7" t="str">
+      <c r="Y24" s="7">
         <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="Z24" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="7">
         <f t="shared" ca="1" si="30"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AA24" s="7" t="str">
         <f t="shared" ca="1" si="30"/>
@@ -6318,13 +6337,13 @@
     </row>
     <row r="25" spans="1:79" s="2" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="8" t="str">
         <f t="shared" ref="I25:BB25" si="32">IF(AND(I$5&gt;=$F22,I$5&lt;=$G22),1,"")</f>
         <v/>
@@ -6345,25 +6364,25 @@
         <f t="shared" si="32"/>
         <v/>
       </c>
-      <c r="N25" s="8">
+      <c r="N25" s="8" t="str">
         <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="O25" s="8">
+        <v/>
+      </c>
+      <c r="O25" s="8" t="str">
         <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="P25" s="8">
+        <v/>
+      </c>
+      <c r="P25" s="8" t="str">
         <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="Q25" s="8">
+        <v/>
+      </c>
+      <c r="Q25" s="8" t="str">
         <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="R25" s="8">
+        <v/>
+      </c>
+      <c r="R25" s="8" t="str">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="S25" s="8">
         <f t="shared" si="32"/>
@@ -6389,13 +6408,13 @@
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
-      <c r="Y25" s="8" t="str">
+      <c r="Y25" s="8">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="Z25" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="8">
         <f t="shared" si="32"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AA25" s="8" t="str">
         <f t="shared" si="32"/>
@@ -6576,21 +6595,21 @@
     </row>
     <row r="26" spans="1:79" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="24" t="s">
+      <c r="B26" s="28"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="27">
-        <f>G22</f>
+      <c r="F26" s="18">
+        <f>G22-2</f>
         <v>44671</v>
       </c>
-      <c r="G26" s="27">
-        <f>F26 + 7</f>
-        <v>44678</v>
-      </c>
-      <c r="H26" s="27"/>
+      <c r="G26" s="18">
+        <f>F26 + 3</f>
+        <v>44674</v>
+      </c>
+      <c r="H26" s="18"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
@@ -6665,13 +6684,13 @@
     </row>
     <row r="27" spans="1:79" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
       <c r="I27" s="7" t="str">
         <f t="shared" ref="I27:BO27" si="34">IF(AND(I$5&gt;=$F26,I$5&lt;=$G26),1,"")</f>
         <v/>
@@ -6748,21 +6767,21 @@
         <f t="shared" si="34"/>
         <v>1</v>
       </c>
-      <c r="AB27" s="7">
+      <c r="AB27" s="7" t="str">
         <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="AC27" s="7">
+        <v/>
+      </c>
+      <c r="AC27" s="7" t="str">
         <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="AD27" s="7">
+        <v/>
+      </c>
+      <c r="AD27" s="7" t="str">
         <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="AE27" s="7">
+        <v/>
+      </c>
+      <c r="AE27" s="7" t="str">
         <f t="shared" si="34"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="AF27" s="7" t="str">
         <f t="shared" si="34"/>
@@ -6923,13 +6942,13 @@
     </row>
     <row r="28" spans="1:79" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
       <c r="I28" s="7" t="str">
         <f t="shared" ref="I28:BO28" ca="1" si="35">IF(OR($H26&gt;I$5,$H26=""),IF(AND(I$5&gt;=$F26,I$5&lt;=$C$3),2,IF(AND(I$5&gt;=$F26,I$5&lt;=$G26),1,"")), IF($H26=I$5,3,I29))</f>
         <v/>
@@ -7006,21 +7025,21 @@
         <f t="shared" ca="1" si="35"/>
         <v>1</v>
       </c>
-      <c r="AB28" s="7">
+      <c r="AB28" s="7" t="str">
         <f t="shared" ca="1" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="AC28" s="7">
+        <v/>
+      </c>
+      <c r="AC28" s="7" t="str">
         <f t="shared" ca="1" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="AD28" s="7">
+        <v/>
+      </c>
+      <c r="AD28" s="7" t="str">
         <f t="shared" ca="1" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="AE28" s="7">
+        <v/>
+      </c>
+      <c r="AE28" s="7" t="str">
         <f t="shared" ca="1" si="35"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="AF28" s="7" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -7181,13 +7200,13 @@
     </row>
     <row r="29" spans="1:79" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
       <c r="I29" s="8" t="str">
         <f t="shared" ref="I29:BB29" si="36">IF(AND(I$5&gt;=$F26,I$5&lt;=$G26),1,"")</f>
         <v/>
@@ -7264,21 +7283,21 @@
         <f t="shared" si="36"/>
         <v>1</v>
       </c>
-      <c r="AB29" s="8">
+      <c r="AB29" s="8" t="str">
         <f t="shared" si="36"/>
-        <v>1</v>
-      </c>
-      <c r="AC29" s="8">
+        <v/>
+      </c>
+      <c r="AC29" s="8" t="str">
         <f t="shared" si="36"/>
-        <v>1</v>
-      </c>
-      <c r="AD29" s="8">
+        <v/>
+      </c>
+      <c r="AD29" s="8" t="str">
         <f t="shared" si="36"/>
-        <v>1</v>
-      </c>
-      <c r="AE29" s="8">
+        <v/>
+      </c>
+      <c r="AE29" s="8" t="str">
         <f t="shared" si="36"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="AF29" s="8" t="str">
         <f t="shared" si="36"/>
@@ -7439,13 +7458,21 @@
     </row>
     <row r="30" spans="1:79" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="18">
+        <f>G26</f>
+        <v>44674</v>
+      </c>
+      <c r="G30" s="18">
+        <f>F30+2</f>
+        <v>44676</v>
+      </c>
+      <c r="H30" s="18"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
@@ -7520,13 +7547,13 @@
     </row>
     <row r="31" spans="1:79" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
       <c r="I31" s="7" t="str">
         <f t="shared" ref="I31:BO31" si="38">IF(AND(I$5&gt;=$F30,I$5&lt;=$G30),1,"")</f>
         <v/>
@@ -7599,17 +7626,17 @@
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="AA31" s="7" t="str">
+      <c r="AA31" s="7">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="AB31" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AB31" s="7">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="AC31" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AC31" s="7">
         <f t="shared" si="38"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AD31" s="7" t="str">
         <f t="shared" si="38"/>
@@ -7778,44 +7805,44 @@
     </row>
     <row r="32" spans="1:79" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="7">
+      <c r="B32" s="28"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="7" t="str">
         <f t="shared" ref="I32:BO32" ca="1" si="39">IF(OR($H30&gt;I$5,$H30=""),IF(AND(I$5&gt;=$F30,I$5&lt;=$C$3),2,IF(AND(I$5&gt;=$F30,I$5&lt;=$G30),1,"")), IF($H30=I$5,3,I33))</f>
-        <v>2</v>
-      </c>
-      <c r="J32" s="7">
+        <v/>
+      </c>
+      <c r="J32" s="7" t="str">
         <f t="shared" ca="1" si="39"/>
-        <v>2</v>
-      </c>
-      <c r="K32" s="7">
+        <v/>
+      </c>
+      <c r="K32" s="7" t="str">
         <f t="shared" ca="1" si="39"/>
-        <v>2</v>
-      </c>
-      <c r="L32" s="7">
+        <v/>
+      </c>
+      <c r="L32" s="7" t="str">
         <f t="shared" ca="1" si="39"/>
-        <v>2</v>
-      </c>
-      <c r="M32" s="7">
+        <v/>
+      </c>
+      <c r="M32" s="7" t="str">
         <f t="shared" ca="1" si="39"/>
-        <v>2</v>
-      </c>
-      <c r="N32" s="7">
+        <v/>
+      </c>
+      <c r="N32" s="7" t="str">
         <f t="shared" ca="1" si="39"/>
-        <v>2</v>
-      </c>
-      <c r="O32" s="7">
+        <v/>
+      </c>
+      <c r="O32" s="7" t="str">
         <f t="shared" ca="1" si="39"/>
-        <v>2</v>
-      </c>
-      <c r="P32" s="7">
+        <v/>
+      </c>
+      <c r="P32" s="7" t="str">
         <f t="shared" ca="1" si="39"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="Q32" s="7" t="str">
         <f t="shared" ca="1" si="39"/>
@@ -7857,17 +7884,17 @@
         <f t="shared" ca="1" si="39"/>
         <v/>
       </c>
-      <c r="AA32" s="7" t="str">
+      <c r="AA32" s="7">
         <f t="shared" ca="1" si="39"/>
-        <v/>
-      </c>
-      <c r="AB32" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AB32" s="7">
         <f t="shared" ca="1" si="39"/>
-        <v/>
-      </c>
-      <c r="AC32" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AC32" s="7">
         <f t="shared" ca="1" si="39"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AD32" s="7" t="str">
         <f t="shared" ca="1" si="39"/>
@@ -8036,13 +8063,13 @@
     </row>
     <row r="33" spans="1:79" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
       <c r="I33" s="8" t="str">
         <f t="shared" ref="I33:BB33" si="40">IF(AND(I$5&gt;=$F30,I$5&lt;=$G30),1,"")</f>
         <v/>
@@ -8115,17 +8142,17 @@
         <f t="shared" si="40"/>
         <v/>
       </c>
-      <c r="AA33" s="8" t="str">
+      <c r="AA33" s="8">
         <f t="shared" si="40"/>
-        <v/>
-      </c>
-      <c r="AB33" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="AB33" s="8">
         <f t="shared" si="40"/>
-        <v/>
-      </c>
-      <c r="AC33" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="AC33" s="8">
         <f t="shared" si="40"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AD33" s="8" t="str">
         <f t="shared" si="40"/>
@@ -8294,13 +8321,21 @@
     </row>
     <row r="34" spans="1:79" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="18">
+        <f>G30</f>
+        <v>44676</v>
+      </c>
+      <c r="G34" s="18">
+        <f>F34+7</f>
+        <v>44683</v>
+      </c>
+      <c r="H34" s="18"/>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
@@ -8375,13 +8410,13 @@
     </row>
     <row r="35" spans="1:79" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
       <c r="I35" s="7" t="str">
         <f t="shared" ref="I35:BO35" si="42">IF(AND(I$5&gt;=$F34,I$5&lt;=$G34),1,"")</f>
         <v/>
@@ -8462,37 +8497,37 @@
         <f t="shared" si="42"/>
         <v/>
       </c>
-      <c r="AC35" s="7" t="str">
+      <c r="AC35" s="7">
         <f t="shared" si="42"/>
-        <v/>
-      </c>
-      <c r="AD35" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AD35" s="7">
         <f t="shared" si="42"/>
-        <v/>
-      </c>
-      <c r="AE35" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AE35" s="7">
         <f t="shared" si="42"/>
-        <v/>
-      </c>
-      <c r="AF35" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AF35" s="7">
         <f t="shared" si="42"/>
-        <v/>
-      </c>
-      <c r="AG35" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AG35" s="7">
         <f t="shared" si="42"/>
-        <v/>
-      </c>
-      <c r="AH35" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AH35" s="7">
         <f t="shared" si="42"/>
-        <v/>
-      </c>
-      <c r="AI35" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AI35" s="7">
         <f t="shared" si="42"/>
-        <v/>
-      </c>
-      <c r="AJ35" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AJ35" s="7">
         <f t="shared" si="42"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AK35" s="7" t="str">
         <f t="shared" si="42"/>
@@ -8633,44 +8668,44 @@
     </row>
     <row r="36" spans="1:79" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="7">
+      <c r="B36" s="28"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="7" t="str">
         <f t="shared" ref="I36:BO36" ca="1" si="43">IF(OR($H34&gt;I$5,$H34=""),IF(AND(I$5&gt;=$F34,I$5&lt;=$C$3),2,IF(AND(I$5&gt;=$F34,I$5&lt;=$G34),1,"")), IF($H34=I$5,3,I37))</f>
-        <v>2</v>
-      </c>
-      <c r="J36" s="7">
+        <v/>
+      </c>
+      <c r="J36" s="7" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v>2</v>
-      </c>
-      <c r="K36" s="7">
+        <v/>
+      </c>
+      <c r="K36" s="7" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v>2</v>
-      </c>
-      <c r="L36" s="7">
+        <v/>
+      </c>
+      <c r="L36" s="7" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v>2</v>
-      </c>
-      <c r="M36" s="7">
+        <v/>
+      </c>
+      <c r="M36" s="7" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v>2</v>
-      </c>
-      <c r="N36" s="7">
+        <v/>
+      </c>
+      <c r="N36" s="7" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v>2</v>
-      </c>
-      <c r="O36" s="7">
+        <v/>
+      </c>
+      <c r="O36" s="7" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v>2</v>
-      </c>
-      <c r="P36" s="7">
+        <v/>
+      </c>
+      <c r="P36" s="7" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="Q36" s="7" t="str">
         <f t="shared" ca="1" si="43"/>
@@ -8720,37 +8755,37 @@
         <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
-      <c r="AC36" s="7" t="str">
+      <c r="AC36" s="7">
         <f t="shared" ca="1" si="43"/>
-        <v/>
-      </c>
-      <c r="AD36" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AD36" s="7">
         <f t="shared" ca="1" si="43"/>
-        <v/>
-      </c>
-      <c r="AE36" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AE36" s="7">
         <f t="shared" ca="1" si="43"/>
-        <v/>
-      </c>
-      <c r="AF36" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AF36" s="7">
         <f t="shared" ca="1" si="43"/>
-        <v/>
-      </c>
-      <c r="AG36" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AG36" s="7">
         <f t="shared" ca="1" si="43"/>
-        <v/>
-      </c>
-      <c r="AH36" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AH36" s="7">
         <f t="shared" ca="1" si="43"/>
-        <v/>
-      </c>
-      <c r="AI36" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AI36" s="7">
         <f t="shared" ca="1" si="43"/>
-        <v/>
-      </c>
-      <c r="AJ36" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AJ36" s="7">
         <f t="shared" ca="1" si="43"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AK36" s="7" t="str">
         <f t="shared" ca="1" si="43"/>
@@ -8891,13 +8926,13 @@
     </row>
     <row r="37" spans="1:79" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
       <c r="I37" s="8" t="str">
         <f t="shared" ref="I37:BB37" si="44">IF(AND(I$5&gt;=$F34,I$5&lt;=$G34),1,"")</f>
         <v/>
@@ -8978,37 +9013,37 @@
         <f t="shared" si="44"/>
         <v/>
       </c>
-      <c r="AC37" s="8" t="str">
+      <c r="AC37" s="8">
         <f t="shared" si="44"/>
-        <v/>
-      </c>
-      <c r="AD37" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="AD37" s="8">
         <f t="shared" si="44"/>
-        <v/>
-      </c>
-      <c r="AE37" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="AE37" s="8">
         <f t="shared" si="44"/>
-        <v/>
-      </c>
-      <c r="AF37" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="AF37" s="8">
         <f t="shared" si="44"/>
-        <v/>
-      </c>
-      <c r="AG37" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="AG37" s="8">
         <f t="shared" si="44"/>
-        <v/>
-      </c>
-      <c r="AH37" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="AH37" s="8">
         <f t="shared" si="44"/>
-        <v/>
-      </c>
-      <c r="AI37" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="AI37" s="8">
         <f t="shared" si="44"/>
-        <v/>
-      </c>
-      <c r="AJ37" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="AJ37" s="8">
         <f t="shared" si="44"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AK37" s="8" t="str">
         <f t="shared" si="44"/>
@@ -9147,15 +9182,15 @@
       <c r="BZ37" s="3"/>
       <c r="CA37" s="3"/>
     </row>
-    <row r="38" spans="1:79" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:79" s="2" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
@@ -9230,13 +9265,13 @@
     </row>
     <row r="39" spans="1:79" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
       <c r="I39" s="7" t="str">
         <f t="shared" ref="I39:BO39" si="46">IF(AND(I$5&gt;=$F38,I$5&lt;=$G38),1,"")</f>
         <v/>
@@ -9486,15 +9521,15 @@
       <c r="BZ39" s="3"/>
       <c r="CA39" s="3"/>
     </row>
-    <row r="40" spans="1:79" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:79" s="2" customFormat="1" ht="8.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="28"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
       <c r="I40" s="7">
         <f t="shared" ref="I40:BO40" ca="1" si="47">IF(OR($H38&gt;I$5,$H38=""),IF(AND(I$5&gt;=$F38,I$5&lt;=$C$3),2,IF(AND(I$5&gt;=$F38,I$5&lt;=$G38),1,"")), IF($H38=I$5,3,I41))</f>
         <v>2</v>
@@ -9527,33 +9562,33 @@
         <f t="shared" ca="1" si="47"/>
         <v>2</v>
       </c>
-      <c r="Q40" s="7" t="str">
+      <c r="Q40" s="7">
         <f t="shared" ca="1" si="47"/>
-        <v/>
-      </c>
-      <c r="R40" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="R40" s="7">
         <f t="shared" ca="1" si="47"/>
-        <v/>
-      </c>
-      <c r="S40" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="S40" s="7">
         <f t="shared" ca="1" si="47"/>
-        <v/>
-      </c>
-      <c r="T40" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="T40" s="7">
         <f t="shared" ca="1" si="47"/>
-        <v/>
-      </c>
-      <c r="U40" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="U40" s="7">
         <f t="shared" ca="1" si="47"/>
-        <v/>
-      </c>
-      <c r="V40" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="V40" s="7">
         <f t="shared" ca="1" si="47"/>
-        <v/>
-      </c>
-      <c r="W40" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="W40" s="7">
         <f t="shared" ca="1" si="47"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="X40" s="7" t="str">
         <f t="shared" ca="1" si="47"/>
@@ -9744,15 +9779,15 @@
       <c r="BZ40" s="3"/>
       <c r="CA40" s="3"/>
     </row>
-    <row r="41" spans="1:79" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:79" s="2" customFormat="1" ht="5.0999999999999996" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
       <c r="I41" s="8" t="str">
         <f t="shared" ref="I41:BB41" si="48">IF(AND(I$5&gt;=$F38,I$5&lt;=$G38),1,"")</f>
         <v/>
@@ -10002,15 +10037,15 @@
       <c r="BZ41" s="3"/>
       <c r="CA41" s="3"/>
     </row>
-    <row r="42" spans="1:79" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:79" s="2" customFormat="1" ht="8.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
       <c r="I42" s="7"/>
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
@@ -10083,15 +10118,15 @@
       <c r="BZ42" s="3"/>
       <c r="CA42" s="3"/>
     </row>
-    <row r="43" spans="1:79" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:79" s="2" customFormat="1" ht="5.0999999999999996" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
-      <c r="B43" s="31"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="28"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
       <c r="I43" s="7" t="str">
         <f t="shared" ref="I43:BO43" si="50">IF(AND(I$5&gt;=$F42,I$5&lt;=$G42),1,"")</f>
         <v/>
@@ -10341,15 +10376,15 @@
       <c r="BZ43" s="3"/>
       <c r="CA43" s="3"/>
     </row>
-    <row r="44" spans="1:79" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:79" s="2" customFormat="1" ht="8.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
       <c r="I44" s="7">
         <f t="shared" ref="I44:BO44" ca="1" si="51">IF(OR($H42&gt;I$5,$H42=""),IF(AND(I$5&gt;=$F42,I$5&lt;=$C$3),2,IF(AND(I$5&gt;=$F42,I$5&lt;=$G42),1,"")), IF($H42=I$5,3,I45))</f>
         <v>2</v>
@@ -10382,33 +10417,33 @@
         <f t="shared" ca="1" si="51"/>
         <v>2</v>
       </c>
-      <c r="Q44" s="7" t="str">
+      <c r="Q44" s="7">
         <f t="shared" ca="1" si="51"/>
-        <v/>
-      </c>
-      <c r="R44" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="R44" s="7">
         <f t="shared" ca="1" si="51"/>
-        <v/>
-      </c>
-      <c r="S44" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="S44" s="7">
         <f t="shared" ca="1" si="51"/>
-        <v/>
-      </c>
-      <c r="T44" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="T44" s="7">
         <f t="shared" ca="1" si="51"/>
-        <v/>
-      </c>
-      <c r="U44" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="U44" s="7">
         <f t="shared" ca="1" si="51"/>
-        <v/>
-      </c>
-      <c r="V44" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="V44" s="7">
         <f t="shared" ca="1" si="51"/>
-        <v/>
-      </c>
-      <c r="W44" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="W44" s="7">
         <f t="shared" ca="1" si="51"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="X44" s="7" t="str">
         <f t="shared" ca="1" si="51"/>
@@ -10599,15 +10634,15 @@
       <c r="BZ44" s="3"/>
       <c r="CA44" s="3"/>
     </row>
-    <row r="45" spans="1:79" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:79" s="2" customFormat="1" ht="5.0999999999999996" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
       <c r="I45" s="8" t="str">
         <f t="shared" ref="I45:BB45" si="52">IF(AND(I$5&gt;=$F42,I$5&lt;=$G42),1,"")</f>
         <v/>
@@ -10880,41 +10915,10 @@
     <row r="66" x14ac:dyDescent="0.25"/>
     <row r="67" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="52">
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="D6:D45"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="E42:E45"/>
-    <mergeCell ref="F42:F45"/>
-    <mergeCell ref="G42:G45"/>
-    <mergeCell ref="H42:H45"/>
+  <mergeCells count="53">
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="B1:E1"/>
     <mergeCell ref="B6:B45"/>
     <mergeCell ref="H34:H37"/>
     <mergeCell ref="C38:C41"/>
@@ -10931,8 +10935,40 @@
     <mergeCell ref="C26:C29"/>
     <mergeCell ref="E26:E29"/>
     <mergeCell ref="F26:F29"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="E42:E45"/>
+    <mergeCell ref="F42:F45"/>
+    <mergeCell ref="G42:G45"/>
+    <mergeCell ref="H42:H45"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="D6:D45"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="H10:H13"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:F2 C3:D3 B5:DM5 I10:DM13">
     <cfRule type="cellIs" dxfId="72" priority="157" operator="equal">
@@ -11300,7 +11336,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="BC10:BO11 BC13:BO13" formula="1"/>
   </ignoredErrors>

</xml_diff>